<commit_message>
added support for split column WG format, renamed data files
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/[English_WS].xlsx
+++ b/raw_data/English_WS/[English_WS].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -3384,18 +3384,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2032"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">

</xml_diff>

<commit_message>
added definitions for grammar items
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/[English_WS].xlsx
+++ b/raw_data/English_WS/[English_WS].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5916" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6029" uniqueCount="970">
   <si>
     <t>meow</t>
   </si>
@@ -2797,6 +2797,138 @@
   </si>
   <si>
     <t>time_words</t>
+  </si>
+  <si>
+    <t>does your child ever talk about past events or people who are not present?</t>
+  </si>
+  <si>
+    <t>does your child ever talk about something that's going to happen in the future?</t>
+  </si>
+  <si>
+    <t>does your child talk a bout objects that are not present?</t>
+  </si>
+  <si>
+    <t>does your child understand if you ask for something that is not in the room?</t>
+  </si>
+  <si>
+    <t>does your child ever pick up or point to an object and name an absent person to whom the object belongs?</t>
+  </si>
+  <si>
+    <t>childrens</t>
+  </si>
+  <si>
+    <t>has your child begun to combine word yet?</t>
+  </si>
+  <si>
+    <t>two shoe / two shoes</t>
+  </si>
+  <si>
+    <t>two foot / two feet</t>
+  </si>
+  <si>
+    <t>daddy car / daddy's car</t>
+  </si>
+  <si>
+    <t>kitty sleep / kitty sleeping</t>
+  </si>
+  <si>
+    <t>I make tower / I making tower</t>
+  </si>
+  <si>
+    <t>I fall down / I fell down</t>
+  </si>
+  <si>
+    <t>more cookie / more cookies</t>
+  </si>
+  <si>
+    <t>these my tooth / these my teeth</t>
+  </si>
+  <si>
+    <t>baby blanket / baby's blanket</t>
+  </si>
+  <si>
+    <t>doggie kiss me / doggie kissed me</t>
+  </si>
+  <si>
+    <t>daddy pick me up / daddy picked me up</t>
+  </si>
+  <si>
+    <t>kitty go away / kitty went away</t>
+  </si>
+  <si>
+    <t>doggie table / doggie on table</t>
+  </si>
+  <si>
+    <t>that my truck / that's my truck</t>
+  </si>
+  <si>
+    <t>baby crying / baby is crying</t>
+  </si>
+  <si>
+    <t>you fix it / can you fix it</t>
+  </si>
+  <si>
+    <t>no wash dolly / don't wash dolly</t>
+  </si>
+  <si>
+    <t>want more juice / want juice in there</t>
+  </si>
+  <si>
+    <t>there a kitty / there's a kitty</t>
+  </si>
+  <si>
+    <t>go bye-bye / wanna go bye-bye</t>
+  </si>
+  <si>
+    <t>where mommy go / where did mommy go</t>
+  </si>
+  <si>
+    <t>coffee hot / that coffee hot</t>
+  </si>
+  <si>
+    <t>I no do it / I can't do it</t>
+  </si>
+  <si>
+    <t>I like read stories / I like to read stories</t>
+  </si>
+  <si>
+    <t>don't read book / don't want you read that book</t>
+  </si>
+  <si>
+    <t>turn on light / turn on light so I can see</t>
+  </si>
+  <si>
+    <t>I want that / I want that one you got</t>
+  </si>
+  <si>
+    <t>want cookies / want cookies and milk</t>
+  </si>
+  <si>
+    <t>cookie mommy / cookie for mommy</t>
+  </si>
+  <si>
+    <t>baby want eat / baby want to eat</t>
+  </si>
+  <si>
+    <t>lookit me / lookit me dancing</t>
+  </si>
+  <si>
+    <t>lookit / lookit what I got</t>
+  </si>
+  <si>
+    <t>where's my dolly / where's my dolly name Sam</t>
+  </si>
+  <si>
+    <t>read me story, Mommy / read me a story, Mommy</t>
+  </si>
+  <si>
+    <t>we made this / me and Paul made this</t>
+  </si>
+  <si>
+    <t>I sing song / I sing song for you</t>
+  </si>
+  <si>
+    <t>baby crying / baby crying cuz she's sad</t>
   </si>
 </sst>
 </file>
@@ -2904,8 +3036,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3026,7 +3160,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3070,6 +3204,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3113,6 +3248,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3444,8 +3580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C404" sqref="C404"/>
+    <sheetView tabSelected="1" topLeftCell="A777" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G799" sqref="G799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3456,7 +3592,7 @@
     <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21166,7 +21302,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="682" spans="1:8">
+    <row r="682" spans="1:8" ht="28">
       <c r="A682" s="12" t="s">
         <v>762</v>
       </c>
@@ -21181,9 +21317,11 @@
       </c>
       <c r="E682" s="10"/>
       <c r="F682" s="13"/>
-      <c r="G682" s="13"/>
-    </row>
-    <row r="683" spans="1:8">
+      <c r="G682" s="13" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="683" spans="1:8" ht="28">
       <c r="A683" s="12" t="s">
         <v>906</v>
       </c>
@@ -21198,9 +21336,11 @@
       </c>
       <c r="E683" s="10"/>
       <c r="F683" s="13"/>
-      <c r="G683" s="13"/>
-    </row>
-    <row r="684" spans="1:8">
+      <c r="G683" s="13" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="684" spans="1:8" ht="28">
       <c r="A684" s="12" t="s">
         <v>907</v>
       </c>
@@ -21215,9 +21355,11 @@
       </c>
       <c r="E684" s="10"/>
       <c r="F684" s="13"/>
-      <c r="G684" s="13"/>
-    </row>
-    <row r="685" spans="1:8">
+      <c r="G684" s="13" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="685" spans="1:8" ht="28">
       <c r="A685" s="12" t="s">
         <v>908</v>
       </c>
@@ -21232,9 +21374,11 @@
       </c>
       <c r="E685" s="10"/>
       <c r="F685" s="13"/>
-      <c r="G685" s="13"/>
-    </row>
-    <row r="686" spans="1:8">
+      <c r="G685" s="13" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="686" spans="1:8" ht="42">
       <c r="A686" s="12" t="s">
         <v>905</v>
       </c>
@@ -21249,7 +21393,9 @@
       </c>
       <c r="E686" s="10"/>
       <c r="F686" s="13"/>
-      <c r="G686" s="13"/>
+      <c r="G686" s="13" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="687" spans="1:8">
       <c r="A687" s="12" t="s">
@@ -21334,7 +21480,9 @@
       </c>
       <c r="E691" s="10"/>
       <c r="F691" s="13"/>
-      <c r="G691" s="13"/>
+      <c r="G691" s="11" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="692" spans="1:7">
       <c r="A692" s="11" t="s">
@@ -21351,7 +21499,9 @@
       </c>
       <c r="E692" s="10"/>
       <c r="F692" s="13"/>
-      <c r="G692" s="13"/>
+      <c r="G692" s="11" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="693" spans="1:7">
       <c r="A693" s="11" t="s">
@@ -21368,7 +21518,9 @@
       </c>
       <c r="E693" s="10"/>
       <c r="F693" s="13"/>
-      <c r="G693" s="13"/>
+      <c r="G693" s="11" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="694" spans="1:7">
       <c r="A694" s="11" t="s">
@@ -21385,7 +21537,9 @@
       </c>
       <c r="E694" s="10"/>
       <c r="F694" s="13"/>
-      <c r="G694" s="13"/>
+      <c r="G694" s="11" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="695" spans="1:7">
       <c r="A695" s="11" t="s">
@@ -21402,7 +21556,9 @@
       </c>
       <c r="E695" s="10"/>
       <c r="F695" s="13"/>
-      <c r="G695" s="13"/>
+      <c r="G695" s="11" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="696" spans="1:7">
       <c r="A696" s="11" t="s">
@@ -21419,7 +21575,9 @@
       </c>
       <c r="E696" s="10"/>
       <c r="F696" s="13"/>
-      <c r="G696" s="13"/>
+      <c r="G696" s="11" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="697" spans="1:7">
       <c r="A697" s="11" t="s">
@@ -21436,7 +21594,9 @@
       </c>
       <c r="E697" s="10"/>
       <c r="F697" s="13"/>
-      <c r="G697" s="13"/>
+      <c r="G697" s="11" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="698" spans="1:7">
       <c r="A698" s="11" t="s">
@@ -21453,7 +21613,9 @@
       </c>
       <c r="E698" s="10"/>
       <c r="F698" s="13"/>
-      <c r="G698" s="13"/>
+      <c r="G698" s="11" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="699" spans="1:7">
       <c r="A699" s="11" t="s">
@@ -21470,7 +21632,9 @@
       </c>
       <c r="E699" s="10"/>
       <c r="F699" s="13"/>
-      <c r="G699" s="13"/>
+      <c r="G699" s="11" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="700" spans="1:7">
       <c r="A700" s="11" t="s">
@@ -21487,7 +21651,9 @@
       </c>
       <c r="E700" s="10"/>
       <c r="F700" s="13"/>
-      <c r="G700" s="13"/>
+      <c r="G700" s="11" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="701" spans="1:7">
       <c r="A701" s="11" t="s">
@@ -21504,7 +21670,9 @@
       </c>
       <c r="E701" s="10"/>
       <c r="F701" s="13"/>
-      <c r="G701" s="13"/>
+      <c r="G701" s="11" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="702" spans="1:7">
       <c r="A702" s="11" t="s">
@@ -21521,7 +21689,9 @@
       </c>
       <c r="E702" s="10"/>
       <c r="F702" s="13"/>
-      <c r="G702" s="13"/>
+      <c r="G702" s="11" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="703" spans="1:7">
       <c r="A703" s="11" t="s">
@@ -21538,7 +21708,9 @@
       </c>
       <c r="E703" s="10"/>
       <c r="F703" s="13"/>
-      <c r="G703" s="13"/>
+      <c r="G703" s="11" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="704" spans="1:7">
       <c r="A704" s="11" t="s">
@@ -21555,7 +21727,9 @@
       </c>
       <c r="E704" s="10"/>
       <c r="F704" s="13"/>
-      <c r="G704" s="13"/>
+      <c r="G704" s="11" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="705" spans="1:7">
       <c r="A705" s="11" t="s">
@@ -21572,7 +21746,9 @@
       </c>
       <c r="E705" s="10"/>
       <c r="F705" s="13"/>
-      <c r="G705" s="13"/>
+      <c r="G705" s="11" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="706" spans="1:7">
       <c r="A706" s="11" t="s">
@@ -21589,7 +21765,9 @@
       </c>
       <c r="E706" s="10"/>
       <c r="F706" s="13"/>
-      <c r="G706" s="13"/>
+      <c r="G706" s="11" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="707" spans="1:7">
       <c r="A707" s="11" t="s">
@@ -21606,7 +21784,9 @@
       </c>
       <c r="E707" s="10"/>
       <c r="F707" s="13"/>
-      <c r="G707" s="13"/>
+      <c r="G707" s="11" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="708" spans="1:7">
       <c r="A708" s="11" t="s">
@@ -21623,7 +21803,9 @@
       </c>
       <c r="E708" s="10"/>
       <c r="F708" s="13"/>
-      <c r="G708" s="13"/>
+      <c r="G708" s="11" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="709" spans="1:7">
       <c r="A709" s="11" t="s">
@@ -21640,7 +21822,9 @@
       </c>
       <c r="E709" s="10"/>
       <c r="F709" s="13"/>
-      <c r="G709" s="13"/>
+      <c r="G709" s="11" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="710" spans="1:7">
       <c r="A710" s="11" t="s">
@@ -21657,7 +21841,9 @@
       </c>
       <c r="E710" s="10"/>
       <c r="F710" s="13"/>
-      <c r="G710" s="13"/>
+      <c r="G710" s="11" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="711" spans="1:7">
       <c r="A711" s="11" t="s">
@@ -21674,7 +21860,9 @@
       </c>
       <c r="E711" s="10"/>
       <c r="F711" s="13"/>
-      <c r="G711" s="13"/>
+      <c r="G711" s="11" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="712" spans="1:7">
       <c r="A712" s="11" t="s">
@@ -21691,7 +21879,9 @@
       </c>
       <c r="E712" s="10"/>
       <c r="F712" s="13"/>
-      <c r="G712" s="13"/>
+      <c r="G712" s="11" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="713" spans="1:7">
       <c r="A713" s="11" t="s">
@@ -21708,7 +21898,9 @@
       </c>
       <c r="E713" s="10"/>
       <c r="F713" s="13"/>
-      <c r="G713" s="13"/>
+      <c r="G713" s="11" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="714" spans="1:7">
       <c r="A714" s="11" t="s">
@@ -21725,7 +21917,9 @@
       </c>
       <c r="E714" s="10"/>
       <c r="F714" s="13"/>
-      <c r="G714" s="13"/>
+      <c r="G714" s="11" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="715" spans="1:7">
       <c r="A715" s="11" t="s">
@@ -21742,7 +21936,9 @@
       </c>
       <c r="E715" s="10"/>
       <c r="F715" s="13"/>
-      <c r="G715" s="13"/>
+      <c r="G715" s="11" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="716" spans="1:7">
       <c r="A716" s="11" t="s">
@@ -21759,7 +21955,9 @@
       </c>
       <c r="E716" s="10"/>
       <c r="F716" s="13"/>
-      <c r="G716" s="13"/>
+      <c r="G716" s="11" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="717" spans="1:7">
       <c r="A717" s="11" t="s">
@@ -21776,7 +21974,9 @@
       </c>
       <c r="E717" s="10"/>
       <c r="F717" s="13"/>
-      <c r="G717" s="13"/>
+      <c r="G717" s="11" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="718" spans="1:7">
       <c r="A718" s="11" t="s">
@@ -21793,7 +21993,9 @@
       </c>
       <c r="E718" s="10"/>
       <c r="F718" s="13"/>
-      <c r="G718" s="13"/>
+      <c r="G718" s="11" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="719" spans="1:7">
       <c r="A719" s="11" t="s">
@@ -21810,7 +22012,9 @@
       </c>
       <c r="E719" s="10"/>
       <c r="F719" s="13"/>
-      <c r="G719" s="13"/>
+      <c r="G719" s="11" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="720" spans="1:7">
       <c r="A720" s="11" t="s">
@@ -21827,7 +22031,9 @@
       </c>
       <c r="E720" s="10"/>
       <c r="F720" s="13"/>
-      <c r="G720" s="13"/>
+      <c r="G720" s="11" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="721" spans="1:7">
       <c r="A721" s="11" t="s">
@@ -21844,7 +22050,9 @@
       </c>
       <c r="E721" s="10"/>
       <c r="F721" s="13"/>
-      <c r="G721" s="13"/>
+      <c r="G721" s="11" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="722" spans="1:7">
       <c r="A722" s="11" t="s">
@@ -21861,7 +22069,9 @@
       </c>
       <c r="E722" s="10"/>
       <c r="F722" s="13"/>
-      <c r="G722" s="13"/>
+      <c r="G722" s="11" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="723" spans="1:7">
       <c r="A723" s="11" t="s">
@@ -21878,7 +22088,9 @@
       </c>
       <c r="E723" s="10"/>
       <c r="F723" s="13"/>
-      <c r="G723" s="13"/>
+      <c r="G723" s="11" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="724" spans="1:7">
       <c r="A724" s="11" t="s">
@@ -21895,7 +22107,9 @@
       </c>
       <c r="E724" s="10"/>
       <c r="F724" s="13"/>
-      <c r="G724" s="13"/>
+      <c r="G724" s="11" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="725" spans="1:7">
       <c r="A725" s="11" t="s">
@@ -21912,7 +22126,9 @@
       </c>
       <c r="E725" s="10"/>
       <c r="F725" s="13"/>
-      <c r="G725" s="13"/>
+      <c r="G725" s="11" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="726" spans="1:7">
       <c r="A726" s="11" t="s">
@@ -21929,7 +22145,9 @@
       </c>
       <c r="E726" s="10"/>
       <c r="F726" s="13"/>
-      <c r="G726" s="13"/>
+      <c r="G726" s="11" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="727" spans="1:7">
       <c r="A727" s="11" t="s">
@@ -21946,7 +22164,9 @@
       </c>
       <c r="E727" s="10"/>
       <c r="F727" s="13"/>
-      <c r="G727" s="13"/>
+      <c r="G727" s="11" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="728" spans="1:7">
       <c r="A728" s="11" t="s">
@@ -21963,7 +22183,9 @@
       </c>
       <c r="E728" s="10"/>
       <c r="F728" s="13"/>
-      <c r="G728" s="13"/>
+      <c r="G728" s="11" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="729" spans="1:7">
       <c r="A729" s="11" t="s">
@@ -21980,7 +22202,9 @@
       </c>
       <c r="E729" s="10"/>
       <c r="F729" s="13"/>
-      <c r="G729" s="13"/>
+      <c r="G729" s="11" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="730" spans="1:7">
       <c r="A730" s="11" t="s">
@@ -21997,7 +22221,9 @@
       </c>
       <c r="E730" s="10"/>
       <c r="F730" s="13"/>
-      <c r="G730" s="13"/>
+      <c r="G730" s="11" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="731" spans="1:7">
       <c r="A731" s="11" t="s">
@@ -22014,7 +22240,9 @@
       </c>
       <c r="E731" s="10"/>
       <c r="F731" s="13"/>
-      <c r="G731" s="13"/>
+      <c r="G731" s="11" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="732" spans="1:7">
       <c r="A732" s="11" t="s">
@@ -22031,7 +22259,9 @@
       </c>
       <c r="E732" s="10"/>
       <c r="F732" s="13"/>
-      <c r="G732" s="13"/>
+      <c r="G732" s="11" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="733" spans="1:7">
       <c r="A733" s="11" t="s">
@@ -22048,7 +22278,9 @@
       </c>
       <c r="E733" s="10"/>
       <c r="F733" s="13"/>
-      <c r="G733" s="13"/>
+      <c r="G733" s="11" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="734" spans="1:7">
       <c r="A734" s="11" t="s">
@@ -22065,7 +22297,9 @@
       </c>
       <c r="E734" s="10"/>
       <c r="F734" s="13"/>
-      <c r="G734" s="13"/>
+      <c r="G734" s="11" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="735" spans="1:7">
       <c r="A735" s="11" t="s">
@@ -22082,7 +22316,9 @@
       </c>
       <c r="E735" s="10"/>
       <c r="F735" s="13"/>
-      <c r="G735" s="13"/>
+      <c r="G735" s="11" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="736" spans="1:7">
       <c r="A736" s="11" t="s">
@@ -22099,7 +22335,9 @@
       </c>
       <c r="E736" s="10"/>
       <c r="F736" s="13"/>
-      <c r="G736" s="13"/>
+      <c r="G736" s="11" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="737" spans="1:7">
       <c r="A737" s="11" t="s">
@@ -22116,7 +22354,9 @@
       </c>
       <c r="E737" s="10"/>
       <c r="F737" s="13"/>
-      <c r="G737" s="13"/>
+      <c r="G737" s="11" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="738" spans="1:7">
       <c r="A738" s="11" t="s">
@@ -22133,7 +22373,9 @@
       </c>
       <c r="E738" s="10"/>
       <c r="F738" s="13"/>
-      <c r="G738" s="13"/>
+      <c r="G738" s="11" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="739" spans="1:7">
       <c r="A739" s="11" t="s">
@@ -22150,7 +22392,9 @@
       </c>
       <c r="E739" s="10"/>
       <c r="F739" s="13"/>
-      <c r="G739" s="13"/>
+      <c r="G739" s="11" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="740" spans="1:7">
       <c r="A740" s="11" t="s">
@@ -22167,7 +22411,9 @@
       </c>
       <c r="E740" s="10"/>
       <c r="F740" s="13"/>
-      <c r="G740" s="13"/>
+      <c r="G740" s="11" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="741" spans="1:7">
       <c r="A741" s="11" t="s">
@@ -22184,7 +22430,9 @@
       </c>
       <c r="E741" s="10"/>
       <c r="F741" s="13"/>
-      <c r="G741" s="13"/>
+      <c r="G741" s="11" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="742" spans="1:7">
       <c r="A742" s="11" t="s">
@@ -22201,7 +22449,9 @@
       </c>
       <c r="E742" s="10"/>
       <c r="F742" s="13"/>
-      <c r="G742" s="13"/>
+      <c r="G742" s="11" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="743" spans="1:7">
       <c r="A743" s="11" t="s">
@@ -22218,7 +22468,9 @@
       </c>
       <c r="E743" s="10"/>
       <c r="F743" s="13"/>
-      <c r="G743" s="13"/>
+      <c r="G743" s="11" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="744" spans="1:7">
       <c r="A744" s="11" t="s">
@@ -22235,7 +22487,9 @@
       </c>
       <c r="E744" s="10"/>
       <c r="F744" s="13"/>
-      <c r="G744" s="13"/>
+      <c r="G744" s="11" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="745" spans="1:7">
       <c r="A745" s="11" t="s">
@@ -22252,7 +22506,9 @@
       </c>
       <c r="E745" s="10"/>
       <c r="F745" s="13"/>
-      <c r="G745" s="13"/>
+      <c r="G745" s="11" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="746" spans="1:7">
       <c r="A746" s="11" t="s">
@@ -22269,7 +22525,9 @@
       </c>
       <c r="E746" s="10"/>
       <c r="F746" s="13"/>
-      <c r="G746" s="13"/>
+      <c r="G746" s="11" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="747" spans="1:7">
       <c r="A747" s="11" t="s">
@@ -22286,7 +22544,9 @@
       </c>
       <c r="E747" s="10"/>
       <c r="F747" s="13"/>
-      <c r="G747" s="13"/>
+      <c r="G747" s="11" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="748" spans="1:7">
       <c r="A748" s="11" t="s">
@@ -22303,7 +22563,9 @@
       </c>
       <c r="E748" s="10"/>
       <c r="F748" s="13"/>
-      <c r="G748" s="13"/>
+      <c r="G748" s="11" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="749" spans="1:7">
       <c r="A749" s="11" t="s">
@@ -22320,7 +22582,9 @@
       </c>
       <c r="E749" s="10"/>
       <c r="F749" s="13"/>
-      <c r="G749" s="13"/>
+      <c r="G749" s="11" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="750" spans="1:7">
       <c r="A750" s="11" t="s">
@@ -22337,7 +22601,9 @@
       </c>
       <c r="E750" s="10"/>
       <c r="F750" s="13"/>
-      <c r="G750" s="13"/>
+      <c r="G750" s="11" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="751" spans="1:7">
       <c r="A751" s="11" t="s">
@@ -22354,7 +22620,9 @@
       </c>
       <c r="E751" s="10"/>
       <c r="F751" s="13"/>
-      <c r="G751" s="13"/>
+      <c r="G751" s="11" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="752" spans="1:7">
       <c r="A752" s="11" t="s">
@@ -22371,7 +22639,9 @@
       </c>
       <c r="E752" s="10"/>
       <c r="F752" s="13"/>
-      <c r="G752" s="13"/>
+      <c r="G752" s="11" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="753" spans="1:7">
       <c r="A753" s="11" t="s">
@@ -22388,7 +22658,9 @@
       </c>
       <c r="E753" s="10"/>
       <c r="F753" s="13"/>
-      <c r="G753" s="13"/>
+      <c r="G753" s="11" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="754" spans="1:7">
       <c r="A754" s="11" t="s">
@@ -22405,7 +22677,9 @@
       </c>
       <c r="E754" s="10"/>
       <c r="F754" s="13"/>
-      <c r="G754" s="13"/>
+      <c r="G754" s="11" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="755" spans="1:7">
       <c r="A755" s="11" t="s">
@@ -22422,7 +22696,9 @@
       </c>
       <c r="E755" s="10"/>
       <c r="F755" s="13"/>
-      <c r="G755" s="13"/>
+      <c r="G755" s="11" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="756" spans="1:7">
       <c r="A756" s="11" t="s">
@@ -22439,7 +22715,9 @@
       </c>
       <c r="E756" s="10"/>
       <c r="F756" s="13"/>
-      <c r="G756" s="13"/>
+      <c r="G756" s="11" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="757" spans="1:7">
       <c r="A757" s="11" t="s">
@@ -22456,7 +22734,9 @@
       </c>
       <c r="E757" s="10"/>
       <c r="F757" s="13"/>
-      <c r="G757" s="13"/>
+      <c r="G757" s="11" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="758" spans="1:7">
       <c r="A758" s="11" t="s">
@@ -22473,7 +22753,9 @@
       </c>
       <c r="E758" s="10"/>
       <c r="F758" s="13"/>
-      <c r="G758" s="13"/>
+      <c r="G758" s="11" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="759" spans="1:7">
       <c r="A759" s="11" t="s">
@@ -22490,7 +22772,9 @@
       </c>
       <c r="E759" s="10"/>
       <c r="F759" s="13"/>
-      <c r="G759" s="13"/>
+      <c r="G759" s="11" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="760" spans="1:7">
       <c r="A760" s="11" t="s">
@@ -22507,7 +22791,9 @@
       </c>
       <c r="E760" s="10"/>
       <c r="F760" s="13"/>
-      <c r="G760" s="13"/>
+      <c r="G760" s="11" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="761" spans="1:7">
       <c r="A761" s="10" t="s">
@@ -22524,7 +22810,9 @@
       </c>
       <c r="E761" s="10"/>
       <c r="F761" s="13"/>
-      <c r="G761" s="13"/>
+      <c r="G761" s="13" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="762" spans="1:7">
       <c r="A762" s="11" t="s">
@@ -22541,7 +22829,9 @@
       </c>
       <c r="E762" s="10"/>
       <c r="F762" s="13"/>
-      <c r="G762" s="13"/>
+      <c r="G762" s="13" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="763" spans="1:7">
       <c r="A763" s="11" t="s">
@@ -22558,7 +22848,9 @@
       </c>
       <c r="E763" s="10"/>
       <c r="F763" s="13"/>
-      <c r="G763" s="13"/>
+      <c r="G763" s="13" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="764" spans="1:7">
       <c r="A764" s="11" t="s">
@@ -22575,7 +22867,9 @@
       </c>
       <c r="E764" s="10"/>
       <c r="F764" s="13"/>
-      <c r="G764" s="13"/>
+      <c r="G764" s="13" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="765" spans="1:7">
       <c r="A765" s="11" t="s">
@@ -22592,7 +22886,9 @@
       </c>
       <c r="E765" s="10"/>
       <c r="F765" s="13"/>
-      <c r="G765" s="13"/>
+      <c r="G765" s="13" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="766" spans="1:7">
       <c r="A766" s="11" t="s">
@@ -22609,7 +22905,9 @@
       </c>
       <c r="E766" s="10"/>
       <c r="F766" s="13"/>
-      <c r="G766" s="13"/>
+      <c r="G766" s="13" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="767" spans="1:7">
       <c r="A767" s="11" t="s">
@@ -22626,7 +22924,9 @@
       </c>
       <c r="E767" s="10"/>
       <c r="F767" s="13"/>
-      <c r="G767" s="13"/>
+      <c r="G767" s="13" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="768" spans="1:7">
       <c r="A768" s="11" t="s">
@@ -22643,7 +22943,9 @@
       </c>
       <c r="E768" s="10"/>
       <c r="F768" s="13"/>
-      <c r="G768" s="13"/>
+      <c r="G768" s="13" t="s">
+        <v>939</v>
+      </c>
     </row>
     <row r="769" spans="1:7">
       <c r="A769" s="11" t="s">
@@ -22660,7 +22962,9 @@
       </c>
       <c r="E769" s="10"/>
       <c r="F769" s="13"/>
-      <c r="G769" s="13"/>
+      <c r="G769" s="13" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="770" spans="1:7">
       <c r="A770" s="11" t="s">
@@ -22677,7 +22981,9 @@
       </c>
       <c r="E770" s="10"/>
       <c r="F770" s="13"/>
-      <c r="G770" s="13"/>
+      <c r="G770" s="13" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="771" spans="1:7">
       <c r="A771" s="11" t="s">
@@ -22694,7 +23000,9 @@
       </c>
       <c r="E771" s="10"/>
       <c r="F771" s="13"/>
-      <c r="G771" s="13"/>
+      <c r="G771" s="13" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="772" spans="1:7">
       <c r="A772" s="11" t="s">
@@ -22711,7 +23019,9 @@
       </c>
       <c r="E772" s="10"/>
       <c r="F772" s="13"/>
-      <c r="G772" s="13"/>
+      <c r="G772" s="13" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="773" spans="1:7">
       <c r="A773" s="11" t="s">
@@ -22728,7 +23038,9 @@
       </c>
       <c r="E773" s="10"/>
       <c r="F773" s="13"/>
-      <c r="G773" s="13"/>
+      <c r="G773" s="13" t="s">
+        <v>944</v>
+      </c>
     </row>
     <row r="774" spans="1:7">
       <c r="A774" s="11" t="s">
@@ -22745,7 +23057,9 @@
       </c>
       <c r="E774" s="10"/>
       <c r="F774" s="13"/>
-      <c r="G774" s="13"/>
+      <c r="G774" s="13" t="s">
+        <v>945</v>
+      </c>
     </row>
     <row r="775" spans="1:7">
       <c r="A775" s="11" t="s">
@@ -22762,7 +23076,9 @@
       </c>
       <c r="E775" s="10"/>
       <c r="F775" s="13"/>
-      <c r="G775" s="13"/>
+      <c r="G775" s="13" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="776" spans="1:7">
       <c r="A776" s="11" t="s">
@@ -22779,7 +23095,9 @@
       </c>
       <c r="E776" s="10"/>
       <c r="F776" s="13"/>
-      <c r="G776" s="13"/>
+      <c r="G776" s="13" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="777" spans="1:7">
       <c r="A777" s="11" t="s">
@@ -22796,7 +23114,9 @@
       </c>
       <c r="E777" s="10"/>
       <c r="F777" s="13"/>
-      <c r="G777" s="13"/>
+      <c r="G777" s="13" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="778" spans="1:7">
       <c r="A778" s="11" t="s">
@@ -22813,7 +23133,9 @@
       </c>
       <c r="E778" s="10"/>
       <c r="F778" s="13"/>
-      <c r="G778" s="13"/>
+      <c r="G778" s="13" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="779" spans="1:7">
       <c r="A779" s="11" t="s">
@@ -22830,7 +23152,9 @@
       </c>
       <c r="E779" s="10"/>
       <c r="F779" s="13"/>
-      <c r="G779" s="13"/>
+      <c r="G779" s="13" t="s">
+        <v>949</v>
+      </c>
     </row>
     <row r="780" spans="1:7">
       <c r="A780" s="11" t="s">
@@ -22847,7 +23171,9 @@
       </c>
       <c r="E780" s="10"/>
       <c r="F780" s="13"/>
-      <c r="G780" s="13"/>
+      <c r="G780" s="13" t="s">
+        <v>950</v>
+      </c>
     </row>
     <row r="781" spans="1:7">
       <c r="A781" s="11" t="s">
@@ -22864,7 +23190,9 @@
       </c>
       <c r="E781" s="10"/>
       <c r="F781" s="13"/>
-      <c r="G781" s="13"/>
+      <c r="G781" s="13" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="782" spans="1:7">
       <c r="A782" s="11" t="s">
@@ -22881,7 +23209,9 @@
       </c>
       <c r="E782" s="10"/>
       <c r="F782" s="13"/>
-      <c r="G782" s="13"/>
+      <c r="G782" s="13" t="s">
+        <v>952</v>
+      </c>
     </row>
     <row r="783" spans="1:7">
       <c r="A783" s="11" t="s">
@@ -22898,7 +23228,9 @@
       </c>
       <c r="E783" s="10"/>
       <c r="F783" s="13"/>
-      <c r="G783" s="13"/>
+      <c r="G783" s="13" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="784" spans="1:7">
       <c r="A784" s="11" t="s">
@@ -22915,7 +23247,9 @@
       </c>
       <c r="E784" s="10"/>
       <c r="F784" s="13"/>
-      <c r="G784" s="13"/>
+      <c r="G784" s="13" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="785" spans="1:7">
       <c r="A785" s="11" t="s">
@@ -22932,7 +23266,9 @@
       </c>
       <c r="E785" s="10"/>
       <c r="F785" s="13"/>
-      <c r="G785" s="13"/>
+      <c r="G785" s="13" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="786" spans="1:7">
       <c r="A786" s="11" t="s">
@@ -22949,7 +23285,9 @@
       </c>
       <c r="E786" s="10"/>
       <c r="F786" s="13"/>
-      <c r="G786" s="13"/>
+      <c r="G786" s="13" t="s">
+        <v>956</v>
+      </c>
     </row>
     <row r="787" spans="1:7">
       <c r="A787" s="11" t="s">
@@ -22966,7 +23304,9 @@
       </c>
       <c r="E787" s="10"/>
       <c r="F787" s="13"/>
-      <c r="G787" s="13"/>
+      <c r="G787" s="13" t="s">
+        <v>957</v>
+      </c>
     </row>
     <row r="788" spans="1:7">
       <c r="A788" s="11" t="s">
@@ -22983,7 +23323,9 @@
       </c>
       <c r="E788" s="10"/>
       <c r="F788" s="13"/>
-      <c r="G788" s="13"/>
+      <c r="G788" s="13" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="789" spans="1:7">
       <c r="A789" s="11" t="s">
@@ -23000,7 +23342,9 @@
       </c>
       <c r="E789" s="10"/>
       <c r="F789" s="13"/>
-      <c r="G789" s="13"/>
+      <c r="G789" s="13" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="790" spans="1:7">
       <c r="A790" s="11" t="s">
@@ -23017,7 +23361,9 @@
       </c>
       <c r="E790" s="10"/>
       <c r="F790" s="13"/>
-      <c r="G790" s="13"/>
+      <c r="G790" s="13" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="791" spans="1:7">
       <c r="A791" s="11" t="s">
@@ -23034,7 +23380,9 @@
       </c>
       <c r="E791" s="10"/>
       <c r="F791" s="13"/>
-      <c r="G791" s="13"/>
+      <c r="G791" s="13" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="792" spans="1:7">
       <c r="A792" s="11" t="s">
@@ -23051,7 +23399,9 @@
       </c>
       <c r="E792" s="10"/>
       <c r="F792" s="13"/>
-      <c r="G792" s="13"/>
+      <c r="G792" s="13" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="793" spans="1:7">
       <c r="A793" s="11" t="s">
@@ -23068,7 +23418,9 @@
       </c>
       <c r="E793" s="10"/>
       <c r="F793" s="13"/>
-      <c r="G793" s="13"/>
+      <c r="G793" s="13" t="s">
+        <v>963</v>
+      </c>
     </row>
     <row r="794" spans="1:7">
       <c r="A794" s="11" t="s">
@@ -23085,7 +23437,9 @@
       </c>
       <c r="E794" s="10"/>
       <c r="F794" s="13"/>
-      <c r="G794" s="13"/>
+      <c r="G794" s="13" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="795" spans="1:7">
       <c r="A795" s="11" t="s">
@@ -23102,7 +23456,9 @@
       </c>
       <c r="E795" s="10"/>
       <c r="F795" s="13"/>
-      <c r="G795" s="13"/>
+      <c r="G795" s="13" t="s">
+        <v>965</v>
+      </c>
     </row>
     <row r="796" spans="1:7">
       <c r="A796" s="11" t="s">
@@ -23119,7 +23475,9 @@
       </c>
       <c r="E796" s="10"/>
       <c r="F796" s="13"/>
-      <c r="G796" s="13"/>
+      <c r="G796" s="13" t="s">
+        <v>967</v>
+      </c>
     </row>
     <row r="797" spans="1:7">
       <c r="A797" s="11" t="s">
@@ -23136,7 +23494,9 @@
       </c>
       <c r="E797" s="10"/>
       <c r="F797" s="13"/>
-      <c r="G797" s="13"/>
+      <c r="G797" s="13" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="798" spans="1:7">
       <c r="A798" s="11" t="s">
@@ -23153,7 +23513,9 @@
       </c>
       <c r="E798" s="10"/>
       <c r="F798" s="13"/>
-      <c r="G798" s="13"/>
+      <c r="G798" s="13" t="s">
+        <v>969</v>
+      </c>
     </row>
     <row r="799" spans="1:7">
       <c r="E799" s="2"/>

</xml_diff>

<commit_message>
fixed mismatched English item definitions
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/[English_WS].xlsx
+++ b/raw_data/English_WS/[English_WS].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="13020" yWindow="-21600" windowWidth="19200" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5610" uniqueCount="1765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5610" uniqueCount="1767">
   <si>
     <t>meow</t>
   </si>
@@ -5314,6 +5314,12 @@
   </si>
   <si>
     <t>read me story, Mommy / read me a story, Mommy</t>
+  </si>
+  <si>
+    <t>night night</t>
+  </si>
+  <si>
+    <t>all gone</t>
   </si>
 </sst>
 </file>
@@ -5399,8 +5405,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5527,7 +5535,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5574,6 +5582,7 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5620,6 +5629,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5951,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2032"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A601" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F624" sqref="F624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14911,10 +14921,10 @@
         <v>873</v>
       </c>
       <c r="F389" s="6" t="s">
-        <v>624</v>
+        <v>1765</v>
       </c>
       <c r="G389" s="6" t="s">
-        <v>624</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="390" spans="1:7">
@@ -17579,10 +17589,10 @@
         <v>873</v>
       </c>
       <c r="F505" s="6" t="s">
-        <v>429</v>
+        <v>1766</v>
       </c>
       <c r="G505" s="6" t="s">
-        <v>429</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="506" spans="1:7">

</xml_diff>

<commit_message>
another English WS/WG mapping fix
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/[English_WS].xlsx
+++ b/raw_data/English_WS/[English_WS].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5610" uniqueCount="1767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5610" uniqueCount="1768">
   <si>
     <t>meow</t>
   </si>
@@ -5320,6 +5320,9 @@
   </si>
   <si>
     <t>all gone</t>
+  </si>
+  <si>
+    <t>little (description)</t>
   </si>
 </sst>
 </file>
@@ -5961,8 +5964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A601" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F624" sqref="F624"/>
+    <sheetView tabSelected="1" topLeftCell="A518" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A538" sqref="A538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18348,10 +18351,10 @@
         <v>873</v>
       </c>
       <c r="F538" s="6" t="s">
-        <v>460</v>
+        <v>1767</v>
       </c>
       <c r="G538" s="6" t="s">
-        <v>460</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="539" spans="1:7">

</xml_diff>